<commit_message>
updated draft of figure
</commit_message>
<xml_diff>
--- a/4_aviation/metric_value/data/data.xlsx
+++ b/4_aviation/metric_value/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelweinold/github/phd_publication_figures/4_aviation/metric_value/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37277006-BC4D-BD46-BE59-90F4D68C59F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B54744-3287-0F4E-8576-4E583E1EE9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{AB350C11-2B71-C046-96F8-F69A1FD61988}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="sa_acft" sheetId="2" r:id="rId2"/>
     <sheet name="trendline" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2099,8 +2099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5747829C-E39B-884E-B8F0-D0DA418496D2}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C46"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2612,6 +2612,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C46">
+    <sortCondition ref="A1:A46"/>
+  </sortState>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{3BCF66B1-5034-1D43-89D5-3AED9029175E}"/>
     <hyperlink ref="C3:C46" r:id="rId2" display="https://theicct.org/wp-content/uploads/2021/06/ICCT_Aircraft-FE-Trends_20150902.pdf" xr:uid="{7E6AFD68-89A7-E04A-BF32-DD44AB0EB851}"/>

</xml_diff>